<commit_message>
ajuste estructura look and felt
ajuste estructura look and felt
</commit_message>
<xml_diff>
--- a/fhir/indisa/StructureDefinition-ProfileLocationBuildingKlinic.xlsx
+++ b/fhir/indisa/StructureDefinition-ProfileLocationBuildingKlinic.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3927" uniqueCount="527">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3927" uniqueCount="526">
   <si>
     <t>Path</t>
   </si>
@@ -628,9 +628,6 @@
   </si>
   <si>
     <t>There are many sets  of identifiers.  To perform matching of two identifiers, we need to know what set we're dealing with. The system identifies a particular set of unique identifiers.</t>
-  </si>
-  <si>
-    <t>http://www.minsalud.gov.co/codHabilitacion</t>
   </si>
   <si>
     <t>http://www.acme.com/identifiers/patient</t>
@@ -4630,49 +4627,49 @@
       </c>
       <c r="P27" s="2"/>
       <c r="Q27" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="R27" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="S27" t="s" s="2">
         <v>198</v>
       </c>
-      <c r="R27" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="S27" t="s" s="2">
+      <c r="T27" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="U27" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="V27" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="W27" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="X27" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Y27" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Z27" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AA27" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AB27" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AC27" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AD27" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AE27" t="s" s="2">
         <v>199</v>
-      </c>
-      <c r="T27" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="U27" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="V27" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="W27" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="X27" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="Y27" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="Z27" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AA27" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AB27" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AC27" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AD27" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AE27" t="s" s="2">
-        <v>200</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>39</v>
@@ -4687,7 +4684,7 @@
         <v>58</v>
       </c>
       <c r="AJ27" t="s" s="2">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AK27" t="s" s="2">
         <v>38</v>
@@ -4695,7 +4692,7 @@
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
@@ -4721,13 +4718,13 @@
         <v>48</v>
       </c>
       <c r="K28" t="s" s="2">
+        <v>202</v>
+      </c>
+      <c r="L28" t="s" s="2">
         <v>203</v>
       </c>
-      <c r="L28" t="s" s="2">
+      <c r="M28" t="s" s="2">
         <v>204</v>
-      </c>
-      <c r="M28" t="s" s="2">
-        <v>205</v>
       </c>
       <c r="N28" s="2"/>
       <c r="O28" t="s" s="2">
@@ -4741,43 +4738,43 @@
         <v>38</v>
       </c>
       <c r="S28" t="s" s="2">
+        <v>205</v>
+      </c>
+      <c r="T28" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="U28" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="V28" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="W28" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="X28" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Y28" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Z28" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AA28" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AB28" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AC28" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AD28" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AE28" t="s" s="2">
         <v>206</v>
-      </c>
-      <c r="T28" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="U28" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="V28" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="W28" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="X28" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="Y28" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="Z28" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AA28" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AB28" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AC28" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AD28" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AE28" t="s" s="2">
-        <v>207</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>39</v>
@@ -4792,7 +4789,7 @@
         <v>58</v>
       </c>
       <c r="AJ28" t="s" s="2">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AK28" t="s" s="2">
         <v>38</v>
@@ -4800,7 +4797,7 @@
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
@@ -4823,13 +4820,13 @@
         <v>47</v>
       </c>
       <c r="J29" t="s" s="2">
+        <v>209</v>
+      </c>
+      <c r="K29" t="s" s="2">
         <v>210</v>
       </c>
-      <c r="K29" t="s" s="2">
+      <c r="L29" t="s" s="2">
         <v>211</v>
-      </c>
-      <c r="L29" t="s" s="2">
-        <v>212</v>
       </c>
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
@@ -4880,7 +4877,7 @@
         <v>38</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="AF29" t="s" s="2">
         <v>39</v>
@@ -4895,7 +4892,7 @@
         <v>58</v>
       </c>
       <c r="AJ29" t="s" s="2">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="AK29" t="s" s="2">
         <v>38</v>
@@ -4903,7 +4900,7 @@
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
@@ -4926,16 +4923,16 @@
         <v>47</v>
       </c>
       <c r="J30" t="s" s="2">
+        <v>215</v>
+      </c>
+      <c r="K30" t="s" s="2">
         <v>216</v>
       </c>
-      <c r="K30" t="s" s="2">
+      <c r="L30" t="s" s="2">
         <v>217</v>
       </c>
-      <c r="L30" t="s" s="2">
+      <c r="M30" t="s" s="2">
         <v>218</v>
-      </c>
-      <c r="M30" t="s" s="2">
-        <v>219</v>
       </c>
       <c r="N30" s="2"/>
       <c r="O30" t="s" s="2">
@@ -4985,7 +4982,7 @@
         <v>38</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>39</v>
@@ -5000,7 +4997,7 @@
         <v>58</v>
       </c>
       <c r="AJ30" t="s" s="2">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AK30" t="s" s="2">
         <v>38</v>
@@ -5008,7 +5005,7 @@
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
@@ -5034,10 +5031,10 @@
         <v>66</v>
       </c>
       <c r="K31" t="s" s="2">
+        <v>222</v>
+      </c>
+      <c r="L31" t="s" s="2">
         <v>223</v>
-      </c>
-      <c r="L31" t="s" s="2">
-        <v>224</v>
       </c>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
@@ -5067,11 +5064,11 @@
         <v>126</v>
       </c>
       <c r="X31" t="s" s="2">
+        <v>224</v>
+      </c>
+      <c r="Y31" t="s" s="2">
         <v>225</v>
       </c>
-      <c r="Y31" t="s" s="2">
-        <v>226</v>
-      </c>
       <c r="Z31" t="s" s="2">
         <v>38</v>
       </c>
@@ -5088,7 +5085,7 @@
         <v>38</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>39</v>
@@ -5103,15 +5100,15 @@
         <v>58</v>
       </c>
       <c r="AJ31" t="s" s="2">
+        <v>226</v>
+      </c>
+      <c r="AK31" t="s" s="2">
         <v>227</v>
-      </c>
-      <c r="AK31" t="s" s="2">
-        <v>228</v>
       </c>
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
@@ -5137,13 +5134,13 @@
         <v>144</v>
       </c>
       <c r="K32" t="s" s="2">
+        <v>229</v>
+      </c>
+      <c r="L32" t="s" s="2">
         <v>230</v>
       </c>
-      <c r="L32" t="s" s="2">
+      <c r="M32" t="s" s="2">
         <v>231</v>
-      </c>
-      <c r="M32" t="s" s="2">
-        <v>232</v>
       </c>
       <c r="N32" s="2"/>
       <c r="O32" t="s" s="2">
@@ -5172,11 +5169,11 @@
         <v>70</v>
       </c>
       <c r="X32" t="s" s="2">
+        <v>232</v>
+      </c>
+      <c r="Y32" t="s" s="2">
         <v>233</v>
       </c>
-      <c r="Y32" t="s" s="2">
-        <v>234</v>
-      </c>
       <c r="Z32" t="s" s="2">
         <v>38</v>
       </c>
@@ -5193,7 +5190,7 @@
         <v>38</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="AF32" t="s" s="2">
         <v>39</v>
@@ -5211,12 +5208,12 @@
         <v>114</v>
       </c>
       <c r="AK32" t="s" s="2">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
@@ -5319,7 +5316,7 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
@@ -5424,7 +5421,7 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
@@ -5466,7 +5463,7 @@
       </c>
       <c r="P35" s="2"/>
       <c r="Q35" t="s" s="2">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="R35" t="s" s="2">
         <v>38</v>
@@ -5531,7 +5528,7 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
@@ -5636,7 +5633,7 @@
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
@@ -5741,7 +5738,7 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -5846,7 +5843,7 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -5953,7 +5950,7 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
@@ -5979,13 +5976,13 @@
         <v>48</v>
       </c>
       <c r="K40" t="s" s="2">
+        <v>243</v>
+      </c>
+      <c r="L40" t="s" s="2">
         <v>244</v>
       </c>
-      <c r="L40" t="s" s="2">
+      <c r="M40" t="s" s="2">
         <v>245</v>
-      </c>
-      <c r="M40" t="s" s="2">
-        <v>246</v>
       </c>
       <c r="N40" s="2"/>
       <c r="O40" t="s" s="2">
@@ -6035,7 +6032,7 @@
         <v>38</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>39</v>
@@ -6050,7 +6047,7 @@
         <v>58</v>
       </c>
       <c r="AJ40" t="s" s="2">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="AK40" t="s" s="2">
         <v>38</v>
@@ -6058,7 +6055,7 @@
     </row>
     <row r="41">
       <c r="A41" t="s" s="2">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
@@ -6084,16 +6081,16 @@
         <v>48</v>
       </c>
       <c r="K41" t="s" s="2">
+        <v>248</v>
+      </c>
+      <c r="L41" t="s" s="2">
         <v>249</v>
       </c>
-      <c r="L41" t="s" s="2">
+      <c r="M41" t="s" s="2">
         <v>250</v>
       </c>
-      <c r="M41" t="s" s="2">
+      <c r="N41" t="s" s="2">
         <v>251</v>
-      </c>
-      <c r="N41" t="s" s="2">
-        <v>252</v>
       </c>
       <c r="O41" t="s" s="2">
         <v>38</v>
@@ -6142,7 +6139,7 @@
         <v>38</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>39</v>
@@ -6157,7 +6154,7 @@
         <v>58</v>
       </c>
       <c r="AJ41" t="s" s="2">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="AK41" t="s" s="2">
         <v>38</v>
@@ -6165,7 +6162,7 @@
     </row>
     <row r="42">
       <c r="A42" t="s" s="2">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
@@ -6191,14 +6188,14 @@
         <v>48</v>
       </c>
       <c r="K42" t="s" s="2">
+        <v>253</v>
+      </c>
+      <c r="L42" t="s" s="2">
         <v>254</v>
-      </c>
-      <c r="L42" t="s" s="2">
-        <v>255</v>
       </c>
       <c r="M42" s="2"/>
       <c r="N42" t="s" s="2">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="O42" t="s" s="2">
         <v>38</v>
@@ -6247,7 +6244,7 @@
         <v>38</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>39</v>
@@ -6262,7 +6259,7 @@
         <v>58</v>
       </c>
       <c r="AJ42" t="s" s="2">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="AK42" t="s" s="2">
         <v>38</v>
@@ -6270,7 +6267,7 @@
     </row>
     <row r="43">
       <c r="A43" t="s" s="2">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
@@ -6296,23 +6293,23 @@
         <v>66</v>
       </c>
       <c r="K43" t="s" s="2">
+        <v>258</v>
+      </c>
+      <c r="L43" t="s" s="2">
         <v>259</v>
       </c>
-      <c r="L43" t="s" s="2">
+      <c r="M43" t="s" s="2">
         <v>260</v>
       </c>
-      <c r="M43" t="s" s="2">
+      <c r="N43" t="s" s="2">
         <v>261</v>
-      </c>
-      <c r="N43" t="s" s="2">
-        <v>262</v>
       </c>
       <c r="O43" t="s" s="2">
         <v>38</v>
       </c>
       <c r="P43" s="2"/>
       <c r="Q43" t="s" s="2">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="R43" t="s" s="2">
         <v>38</v>
@@ -6333,10 +6330,10 @@
         <v>126</v>
       </c>
       <c r="X43" t="s" s="2">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="Y43" t="s" s="2">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="Z43" t="s" s="2">
         <v>38</v>
@@ -6354,7 +6351,7 @@
         <v>38</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="AF43" t="s" s="2">
         <v>39</v>
@@ -6369,15 +6366,15 @@
         <v>58</v>
       </c>
       <c r="AJ43" t="s" s="2">
+        <v>264</v>
+      </c>
+      <c r="AK43" t="s" s="2">
         <v>265</v>
-      </c>
-      <c r="AK43" t="s" s="2">
-        <v>266</v>
       </c>
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -6403,10 +6400,10 @@
         <v>132</v>
       </c>
       <c r="K44" t="s" s="2">
+        <v>267</v>
+      </c>
+      <c r="L44" t="s" s="2">
         <v>268</v>
-      </c>
-      <c r="L44" t="s" s="2">
-        <v>269</v>
       </c>
       <c r="M44" s="2"/>
       <c r="N44" s="2"/>
@@ -6436,11 +6433,11 @@
         <v>137</v>
       </c>
       <c r="X44" t="s" s="2">
+        <v>268</v>
+      </c>
+      <c r="Y44" t="s" s="2">
         <v>269</v>
       </c>
-      <c r="Y44" t="s" s="2">
-        <v>270</v>
-      </c>
       <c r="Z44" t="s" s="2">
         <v>38</v>
       </c>
@@ -6457,7 +6454,7 @@
         <v>38</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="AF44" t="s" s="2">
         <v>39</v>
@@ -6472,15 +6469,15 @@
         <v>58</v>
       </c>
       <c r="AJ44" t="s" s="2">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="AK44" t="s" s="2">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
@@ -6583,7 +6580,7 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
@@ -6688,7 +6685,7 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
@@ -6795,7 +6792,7 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
@@ -6898,7 +6895,7 @@
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
@@ -7003,7 +7000,7 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
@@ -7045,7 +7042,7 @@
       </c>
       <c r="P50" s="2"/>
       <c r="Q50" t="s" s="2">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="R50" t="s" s="2">
         <v>38</v>
@@ -7110,7 +7107,7 @@
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
@@ -7215,7 +7212,7 @@
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
@@ -7320,7 +7317,7 @@
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" t="s" s="2">
@@ -7425,7 +7422,7 @@
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" t="s" s="2">
@@ -7532,7 +7529,7 @@
     </row>
     <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" t="s" s="2">
@@ -7639,7 +7636,7 @@
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" t="s" s="2">
@@ -7662,13 +7659,13 @@
         <v>38</v>
       </c>
       <c r="J56" t="s" s="2">
+        <v>284</v>
+      </c>
+      <c r="K56" t="s" s="2">
         <v>285</v>
       </c>
-      <c r="K56" t="s" s="2">
+      <c r="L56" t="s" s="2">
         <v>286</v>
-      </c>
-      <c r="L56" t="s" s="2">
-        <v>287</v>
       </c>
       <c r="M56" s="2"/>
       <c r="N56" s="2"/>
@@ -7719,7 +7716,7 @@
         <v>38</v>
       </c>
       <c r="AE56" t="s" s="2">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="AF56" t="s" s="2">
         <v>39</v>
@@ -7734,7 +7731,7 @@
         <v>58</v>
       </c>
       <c r="AJ56" t="s" s="2">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="AK56" t="s" s="2">
         <v>38</v>
@@ -7742,7 +7739,7 @@
     </row>
     <row r="57" hidden="true">
       <c r="A57" t="s" s="2">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" t="s" s="2">
@@ -7845,7 +7842,7 @@
     </row>
     <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" t="s" s="2">
@@ -7950,7 +7947,7 @@
     </row>
     <row r="59" hidden="true">
       <c r="A59" t="s" s="2">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" t="s" s="2">
@@ -7976,10 +7973,10 @@
         <v>66</v>
       </c>
       <c r="K59" t="s" s="2">
+        <v>291</v>
+      </c>
+      <c r="L59" t="s" s="2">
         <v>292</v>
-      </c>
-      <c r="L59" t="s" s="2">
-        <v>293</v>
       </c>
       <c r="M59" s="2"/>
       <c r="N59" s="2"/>
@@ -7988,7 +7985,7 @@
       </c>
       <c r="P59" s="2"/>
       <c r="Q59" t="s" s="2">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="R59" t="s" s="2">
         <v>38</v>
@@ -8009,43 +8006,43 @@
         <v>126</v>
       </c>
       <c r="X59" t="s" s="2">
+        <v>293</v>
+      </c>
+      <c r="Y59" t="s" s="2">
         <v>294</v>
       </c>
-      <c r="Y59" t="s" s="2">
+      <c r="Z59" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AA59" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AB59" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AC59" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AD59" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AE59" t="s" s="2">
         <v>295</v>
       </c>
-      <c r="Z59" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AA59" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AB59" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AC59" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AD59" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AE59" t="s" s="2">
+      <c r="AF59" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AG59" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="AH59" t="s" s="2">
         <v>296</v>
-      </c>
-      <c r="AF59" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AG59" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AH59" t="s" s="2">
-        <v>297</v>
       </c>
       <c r="AI59" t="s" s="2">
         <v>58</v>
       </c>
       <c r="AJ59" t="s" s="2">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="AK59" t="s" s="2">
         <v>38</v>
@@ -8053,7 +8050,7 @@
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" t="s" s="2">
@@ -8079,16 +8076,16 @@
         <v>48</v>
       </c>
       <c r="K60" t="s" s="2">
+        <v>299</v>
+      </c>
+      <c r="L60" t="s" s="2">
         <v>300</v>
       </c>
-      <c r="L60" t="s" s="2">
+      <c r="M60" t="s" s="2">
         <v>301</v>
       </c>
-      <c r="M60" t="s" s="2">
+      <c r="N60" t="s" s="2">
         <v>302</v>
-      </c>
-      <c r="N60" t="s" s="2">
-        <v>303</v>
       </c>
       <c r="O60" t="s" s="2">
         <v>38</v>
@@ -8137,7 +8134,7 @@
         <v>38</v>
       </c>
       <c r="AE60" t="s" s="2">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="AF60" t="s" s="2">
         <v>39</v>
@@ -8152,7 +8149,7 @@
         <v>58</v>
       </c>
       <c r="AJ60" t="s" s="2">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="AK60" t="s" s="2">
         <v>38</v>
@@ -8160,7 +8157,7 @@
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" t="s" s="2">
@@ -8186,23 +8183,23 @@
         <v>66</v>
       </c>
       <c r="K61" t="s" s="2">
+        <v>306</v>
+      </c>
+      <c r="L61" t="s" s="2">
         <v>307</v>
       </c>
-      <c r="L61" t="s" s="2">
+      <c r="M61" t="s" s="2">
         <v>308</v>
       </c>
-      <c r="M61" t="s" s="2">
+      <c r="N61" t="s" s="2">
         <v>309</v>
-      </c>
-      <c r="N61" t="s" s="2">
-        <v>310</v>
       </c>
       <c r="O61" t="s" s="2">
         <v>38</v>
       </c>
       <c r="P61" s="2"/>
       <c r="Q61" t="s" s="2">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="R61" t="s" s="2">
         <v>38</v>
@@ -8223,28 +8220,28 @@
         <v>126</v>
       </c>
       <c r="X61" t="s" s="2">
+        <v>310</v>
+      </c>
+      <c r="Y61" t="s" s="2">
         <v>311</v>
       </c>
-      <c r="Y61" t="s" s="2">
+      <c r="Z61" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AA61" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AB61" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AC61" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AD61" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AE61" t="s" s="2">
         <v>312</v>
-      </c>
-      <c r="Z61" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AA61" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AB61" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AC61" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AD61" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AE61" t="s" s="2">
-        <v>313</v>
       </c>
       <c r="AF61" t="s" s="2">
         <v>39</v>
@@ -8259,7 +8256,7 @@
         <v>58</v>
       </c>
       <c r="AJ61" t="s" s="2">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="AK61" t="s" s="2">
         <v>38</v>
@@ -8267,7 +8264,7 @@
     </row>
     <row r="62" hidden="true">
       <c r="A62" t="s" s="2">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" t="s" s="2">
@@ -8290,16 +8287,16 @@
         <v>47</v>
       </c>
       <c r="J62" t="s" s="2">
+        <v>315</v>
+      </c>
+      <c r="K62" t="s" s="2">
         <v>316</v>
       </c>
-      <c r="K62" t="s" s="2">
+      <c r="L62" t="s" s="2">
         <v>317</v>
       </c>
-      <c r="L62" t="s" s="2">
+      <c r="M62" t="s" s="2">
         <v>318</v>
-      </c>
-      <c r="M62" t="s" s="2">
-        <v>319</v>
       </c>
       <c r="N62" s="2"/>
       <c r="O62" t="s" s="2">
@@ -8349,7 +8346,7 @@
         <v>38</v>
       </c>
       <c r="AE62" t="s" s="2">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="AF62" t="s" s="2">
         <v>39</v>
@@ -8372,7 +8369,7 @@
     </row>
     <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" t="s" s="2">
@@ -8395,13 +8392,13 @@
         <v>47</v>
       </c>
       <c r="J63" t="s" s="2">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="K63" t="s" s="2">
+        <v>321</v>
+      </c>
+      <c r="L63" t="s" s="2">
         <v>322</v>
-      </c>
-      <c r="L63" t="s" s="2">
-        <v>323</v>
       </c>
       <c r="M63" s="2"/>
       <c r="N63" s="2"/>
@@ -8452,7 +8449,7 @@
         <v>38</v>
       </c>
       <c r="AE63" t="s" s="2">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="AF63" t="s" s="2">
         <v>39</v>
@@ -8467,7 +8464,7 @@
         <v>58</v>
       </c>
       <c r="AJ63" t="s" s="2">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="AK63" t="s" s="2">
         <v>38</v>
@@ -8475,7 +8472,7 @@
     </row>
     <row r="64" hidden="true">
       <c r="A64" t="s" s="2">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" t="s" s="2">
@@ -8498,19 +8495,19 @@
         <v>38</v>
       </c>
       <c r="J64" t="s" s="2">
+        <v>326</v>
+      </c>
+      <c r="K64" t="s" s="2">
         <v>327</v>
       </c>
-      <c r="K64" t="s" s="2">
+      <c r="L64" t="s" s="2">
         <v>328</v>
       </c>
-      <c r="L64" t="s" s="2">
+      <c r="M64" t="s" s="2">
         <v>329</v>
       </c>
-      <c r="M64" t="s" s="2">
+      <c r="N64" t="s" s="2">
         <v>330</v>
-      </c>
-      <c r="N64" t="s" s="2">
-        <v>331</v>
       </c>
       <c r="O64" t="s" s="2">
         <v>38</v>
@@ -8559,7 +8556,7 @@
         <v>38</v>
       </c>
       <c r="AE64" t="s" s="2">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="AF64" t="s" s="2">
         <v>39</v>
@@ -8574,7 +8571,7 @@
         <v>58</v>
       </c>
       <c r="AJ64" t="s" s="2">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="AK64" t="s" s="2">
         <v>38</v>
@@ -8582,7 +8579,7 @@
     </row>
     <row r="65" hidden="true">
       <c r="A65" t="s" s="2">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B65" s="2"/>
       <c r="C65" t="s" s="2">
@@ -8685,7 +8682,7 @@
     </row>
     <row r="66" hidden="true">
       <c r="A66" t="s" s="2">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B66" s="2"/>
       <c r="C66" t="s" s="2">
@@ -8790,7 +8787,7 @@
     </row>
     <row r="67" hidden="true">
       <c r="A67" t="s" s="2">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B67" s="2"/>
       <c r="C67" t="s" s="2">
@@ -8816,29 +8813,29 @@
         <v>66</v>
       </c>
       <c r="K67" t="s" s="2">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="L67" t="s" s="2">
+        <v>335</v>
+      </c>
+      <c r="M67" t="s" s="2">
         <v>336</v>
       </c>
-      <c r="M67" t="s" s="2">
+      <c r="N67" t="s" s="2">
         <v>337</v>
-      </c>
-      <c r="N67" t="s" s="2">
-        <v>338</v>
       </c>
       <c r="O67" t="s" s="2">
         <v>38</v>
       </c>
       <c r="P67" s="2"/>
       <c r="Q67" t="s" s="2">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="R67" t="s" s="2">
         <v>38</v>
       </c>
       <c r="S67" t="s" s="2">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="T67" t="s" s="2">
         <v>38</v>
@@ -8853,28 +8850,28 @@
         <v>126</v>
       </c>
       <c r="X67" t="s" s="2">
+        <v>339</v>
+      </c>
+      <c r="Y67" t="s" s="2">
         <v>340</v>
       </c>
-      <c r="Y67" t="s" s="2">
+      <c r="Z67" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AA67" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AB67" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AC67" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AD67" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AE67" t="s" s="2">
         <v>341</v>
-      </c>
-      <c r="Z67" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AA67" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AB67" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AC67" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AD67" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AE67" t="s" s="2">
-        <v>342</v>
       </c>
       <c r="AF67" t="s" s="2">
         <v>39</v>
@@ -8889,7 +8886,7 @@
         <v>58</v>
       </c>
       <c r="AJ67" t="s" s="2">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="AK67" t="s" s="2">
         <v>38</v>
@@ -8897,7 +8894,7 @@
     </row>
     <row r="68" hidden="true">
       <c r="A68" t="s" s="2">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B68" s="2"/>
       <c r="C68" t="s" s="2">
@@ -8923,13 +8920,13 @@
         <v>66</v>
       </c>
       <c r="K68" t="s" s="2">
+        <v>343</v>
+      </c>
+      <c r="L68" t="s" s="2">
         <v>344</v>
       </c>
-      <c r="L68" t="s" s="2">
+      <c r="M68" t="s" s="2">
         <v>345</v>
-      </c>
-      <c r="M68" t="s" s="2">
-        <v>346</v>
       </c>
       <c r="N68" s="2"/>
       <c r="O68" t="s" s="2">
@@ -8943,7 +8940,7 @@
         <v>38</v>
       </c>
       <c r="S68" t="s" s="2">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="T68" t="s" s="2">
         <v>38</v>
@@ -8958,28 +8955,28 @@
         <v>126</v>
       </c>
       <c r="X68" t="s" s="2">
+        <v>347</v>
+      </c>
+      <c r="Y68" t="s" s="2">
         <v>348</v>
       </c>
-      <c r="Y68" t="s" s="2">
+      <c r="Z68" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AA68" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AB68" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AC68" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AD68" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AE68" t="s" s="2">
         <v>349</v>
-      </c>
-      <c r="Z68" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AA68" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AB68" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AC68" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AD68" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AE68" t="s" s="2">
-        <v>350</v>
       </c>
       <c r="AF68" t="s" s="2">
         <v>39</v>
@@ -8994,7 +8991,7 @@
         <v>58</v>
       </c>
       <c r="AJ68" t="s" s="2">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="AK68" t="s" s="2">
         <v>38</v>
@@ -9002,7 +8999,7 @@
     </row>
     <row r="69" hidden="true">
       <c r="A69" t="s" s="2">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B69" s="2"/>
       <c r="C69" t="s" s="2">
@@ -9028,16 +9025,16 @@
         <v>48</v>
       </c>
       <c r="K69" t="s" s="2">
+        <v>351</v>
+      </c>
+      <c r="L69" t="s" s="2">
         <v>352</v>
       </c>
-      <c r="L69" t="s" s="2">
+      <c r="M69" t="s" s="2">
         <v>353</v>
       </c>
-      <c r="M69" t="s" s="2">
+      <c r="N69" t="s" s="2">
         <v>354</v>
-      </c>
-      <c r="N69" t="s" s="2">
-        <v>355</v>
       </c>
       <c r="O69" t="s" s="2">
         <v>38</v>
@@ -9050,43 +9047,43 @@
         <v>38</v>
       </c>
       <c r="S69" t="s" s="2">
+        <v>355</v>
+      </c>
+      <c r="T69" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="U69" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="V69" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="W69" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="X69" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Y69" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Z69" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AA69" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AB69" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AC69" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AD69" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AE69" t="s" s="2">
         <v>356</v>
-      </c>
-      <c r="T69" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="U69" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="V69" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="W69" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="X69" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="Y69" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="Z69" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AA69" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AB69" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AC69" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AD69" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AE69" t="s" s="2">
-        <v>357</v>
       </c>
       <c r="AF69" t="s" s="2">
         <v>39</v>
@@ -9101,7 +9098,7 @@
         <v>58</v>
       </c>
       <c r="AJ69" t="s" s="2">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="AK69" t="s" s="2">
         <v>38</v>
@@ -9109,7 +9106,7 @@
     </row>
     <row r="70" hidden="true">
       <c r="A70" t="s" s="2">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B70" s="2"/>
       <c r="C70" t="s" s="2">
@@ -9135,10 +9132,10 @@
         <v>48</v>
       </c>
       <c r="K70" t="s" s="2">
+        <v>359</v>
+      </c>
+      <c r="L70" t="s" s="2">
         <v>360</v>
-      </c>
-      <c r="L70" t="s" s="2">
-        <v>361</v>
       </c>
       <c r="M70" s="2"/>
       <c r="N70" s="2"/>
@@ -9153,43 +9150,43 @@
         <v>38</v>
       </c>
       <c r="S70" t="s" s="2">
+        <v>361</v>
+      </c>
+      <c r="T70" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="U70" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="V70" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="W70" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="X70" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Y70" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Z70" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AA70" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AB70" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AC70" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AD70" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AE70" t="s" s="2">
         <v>362</v>
-      </c>
-      <c r="T70" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="U70" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="V70" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="W70" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="X70" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="Y70" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="Z70" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AA70" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AB70" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AC70" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AD70" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AE70" t="s" s="2">
-        <v>363</v>
       </c>
       <c r="AF70" t="s" s="2">
         <v>39</v>
@@ -9204,7 +9201,7 @@
         <v>58</v>
       </c>
       <c r="AJ70" t="s" s="2">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="AK70" t="s" s="2">
         <v>38</v>
@@ -9212,11 +9209,11 @@
     </row>
     <row r="71" hidden="true">
       <c r="A71" t="s" s="2">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B71" s="2"/>
       <c r="C71" t="s" s="2">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D71" s="2"/>
       <c r="E71" t="s" s="2">
@@ -9238,13 +9235,13 @@
         <v>48</v>
       </c>
       <c r="K71" t="s" s="2">
+        <v>366</v>
+      </c>
+      <c r="L71" t="s" s="2">
         <v>367</v>
       </c>
-      <c r="L71" t="s" s="2">
+      <c r="M71" t="s" s="2">
         <v>368</v>
-      </c>
-      <c r="M71" t="s" s="2">
-        <v>369</v>
       </c>
       <c r="N71" s="2"/>
       <c r="O71" t="s" s="2">
@@ -9258,43 +9255,43 @@
         <v>38</v>
       </c>
       <c r="S71" t="s" s="2">
+        <v>369</v>
+      </c>
+      <c r="T71" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="U71" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="V71" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="W71" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="X71" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Y71" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Z71" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AA71" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AB71" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AC71" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AD71" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AE71" t="s" s="2">
         <v>370</v>
-      </c>
-      <c r="T71" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="U71" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="V71" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="W71" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="X71" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="Y71" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="Z71" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AA71" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AB71" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AC71" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AD71" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AE71" t="s" s="2">
-        <v>371</v>
       </c>
       <c r="AF71" t="s" s="2">
         <v>39</v>
@@ -9309,7 +9306,7 @@
         <v>58</v>
       </c>
       <c r="AJ71" t="s" s="2">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="AK71" t="s" s="2">
         <v>38</v>
@@ -9317,11 +9314,11 @@
     </row>
     <row r="72">
       <c r="A72" t="s" s="2">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B72" s="2"/>
       <c r="C72" t="s" s="2">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D72" s="2"/>
       <c r="E72" t="s" s="2">
@@ -9343,13 +9340,13 @@
         <v>48</v>
       </c>
       <c r="K72" t="s" s="2">
+        <v>374</v>
+      </c>
+      <c r="L72" t="s" s="2">
         <v>375</v>
       </c>
-      <c r="L72" t="s" s="2">
+      <c r="M72" t="s" s="2">
         <v>376</v>
-      </c>
-      <c r="M72" t="s" s="2">
-        <v>377</v>
       </c>
       <c r="N72" s="2"/>
       <c r="O72" t="s" s="2">
@@ -9363,43 +9360,43 @@
         <v>38</v>
       </c>
       <c r="S72" t="s" s="2">
+        <v>377</v>
+      </c>
+      <c r="T72" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="U72" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="V72" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="W72" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="X72" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Y72" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Z72" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AA72" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AB72" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AC72" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AD72" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AE72" t="s" s="2">
         <v>378</v>
-      </c>
-      <c r="T72" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="U72" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="V72" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="W72" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="X72" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="Y72" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="Z72" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AA72" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AB72" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AC72" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AD72" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AE72" t="s" s="2">
-        <v>379</v>
       </c>
       <c r="AF72" t="s" s="2">
         <v>39</v>
@@ -9414,7 +9411,7 @@
         <v>58</v>
       </c>
       <c r="AJ72" t="s" s="2">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="AK72" t="s" s="2">
         <v>38</v>
@@ -9422,11 +9419,11 @@
     </row>
     <row r="73" hidden="true">
       <c r="A73" t="s" s="2">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B73" s="2"/>
       <c r="C73" t="s" s="2">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D73" s="2"/>
       <c r="E73" t="s" s="2">
@@ -9448,13 +9445,13 @@
         <v>48</v>
       </c>
       <c r="K73" t="s" s="2">
+        <v>382</v>
+      </c>
+      <c r="L73" t="s" s="2">
         <v>383</v>
       </c>
-      <c r="L73" t="s" s="2">
+      <c r="M73" t="s" s="2">
         <v>384</v>
-      </c>
-      <c r="M73" t="s" s="2">
-        <v>385</v>
       </c>
       <c r="N73" s="2"/>
       <c r="O73" t="s" s="2">
@@ -9504,7 +9501,7 @@
         <v>38</v>
       </c>
       <c r="AE73" t="s" s="2">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="AF73" t="s" s="2">
         <v>39</v>
@@ -9519,7 +9516,7 @@
         <v>58</v>
       </c>
       <c r="AJ73" t="s" s="2">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="AK73" t="s" s="2">
         <v>38</v>
@@ -9527,11 +9524,11 @@
     </row>
     <row r="74" hidden="true">
       <c r="A74" t="s" s="2">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B74" s="2"/>
       <c r="C74" t="s" s="2">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D74" s="2"/>
       <c r="E74" t="s" s="2">
@@ -9553,10 +9550,10 @@
         <v>48</v>
       </c>
       <c r="K74" t="s" s="2">
+        <v>389</v>
+      </c>
+      <c r="L74" t="s" s="2">
         <v>390</v>
-      </c>
-      <c r="L74" t="s" s="2">
-        <v>391</v>
       </c>
       <c r="M74" s="2"/>
       <c r="N74" s="2"/>
@@ -9571,43 +9568,43 @@
         <v>38</v>
       </c>
       <c r="S74" t="s" s="2">
+        <v>391</v>
+      </c>
+      <c r="T74" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="U74" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="V74" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="W74" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="X74" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Y74" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Z74" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AA74" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AB74" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AC74" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AD74" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AE74" t="s" s="2">
         <v>392</v>
-      </c>
-      <c r="T74" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="U74" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="V74" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="W74" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="X74" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="Y74" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="Z74" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AA74" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AB74" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AC74" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AD74" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AE74" t="s" s="2">
-        <v>393</v>
       </c>
       <c r="AF74" t="s" s="2">
         <v>39</v>
@@ -9622,7 +9619,7 @@
         <v>58</v>
       </c>
       <c r="AJ74" t="s" s="2">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="AK74" t="s" s="2">
         <v>38</v>
@@ -9630,7 +9627,7 @@
     </row>
     <row r="75" hidden="true">
       <c r="A75" t="s" s="2">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B75" s="2"/>
       <c r="C75" t="s" s="2">
@@ -9656,13 +9653,13 @@
         <v>48</v>
       </c>
       <c r="K75" t="s" s="2">
+        <v>395</v>
+      </c>
+      <c r="L75" t="s" s="2">
         <v>396</v>
       </c>
-      <c r="L75" t="s" s="2">
+      <c r="M75" t="s" s="2">
         <v>397</v>
-      </c>
-      <c r="M75" t="s" s="2">
-        <v>398</v>
       </c>
       <c r="N75" s="2"/>
       <c r="O75" t="s" s="2">
@@ -9712,7 +9709,7 @@
         <v>38</v>
       </c>
       <c r="AE75" t="s" s="2">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="AF75" t="s" s="2">
         <v>39</v>
@@ -9727,7 +9724,7 @@
         <v>58</v>
       </c>
       <c r="AJ75" t="s" s="2">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="AK75" t="s" s="2">
         <v>38</v>
@@ -9735,7 +9732,7 @@
     </row>
     <row r="76" hidden="true">
       <c r="A76" t="s" s="2">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B76" s="2"/>
       <c r="C76" t="s" s="2">
@@ -9758,17 +9755,17 @@
         <v>47</v>
       </c>
       <c r="J76" t="s" s="2">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="K76" t="s" s="2">
+        <v>401</v>
+      </c>
+      <c r="L76" t="s" s="2">
         <v>402</v>
-      </c>
-      <c r="L76" t="s" s="2">
-        <v>403</v>
       </c>
       <c r="M76" s="2"/>
       <c r="N76" t="s" s="2">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="O76" t="s" s="2">
         <v>38</v>
@@ -9781,43 +9778,43 @@
         <v>38</v>
       </c>
       <c r="S76" t="s" s="2">
+        <v>404</v>
+      </c>
+      <c r="T76" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="U76" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="V76" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="W76" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="X76" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Y76" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Z76" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AA76" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AB76" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AC76" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AD76" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AE76" t="s" s="2">
         <v>405</v>
-      </c>
-      <c r="T76" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="U76" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="V76" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="W76" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="X76" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="Y76" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="Z76" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AA76" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AB76" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AC76" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AD76" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AE76" t="s" s="2">
-        <v>406</v>
       </c>
       <c r="AF76" t="s" s="2">
         <v>39</v>
@@ -9832,7 +9829,7 @@
         <v>58</v>
       </c>
       <c r="AJ76" t="s" s="2">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="AK76" t="s" s="2">
         <v>38</v>
@@ -9840,7 +9837,7 @@
     </row>
     <row r="77" hidden="true">
       <c r="A77" t="s" s="2">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B77" s="2"/>
       <c r="C77" t="s" s="2">
@@ -9866,14 +9863,14 @@
         <v>132</v>
       </c>
       <c r="K77" t="s" s="2">
+        <v>407</v>
+      </c>
+      <c r="L77" t="s" s="2">
         <v>408</v>
-      </c>
-      <c r="L77" t="s" s="2">
-        <v>409</v>
       </c>
       <c r="M77" s="2"/>
       <c r="N77" t="s" s="2">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="O77" t="s" s="2">
         <v>38</v>
@@ -9898,14 +9895,14 @@
         <v>38</v>
       </c>
       <c r="W77" t="s" s="2">
+        <v>410</v>
+      </c>
+      <c r="X77" t="s" s="2">
         <v>411</v>
       </c>
-      <c r="X77" t="s" s="2">
+      <c r="Y77" t="s" s="2">
         <v>412</v>
       </c>
-      <c r="Y77" t="s" s="2">
-        <v>413</v>
-      </c>
       <c r="Z77" t="s" s="2">
         <v>38</v>
       </c>
@@ -9922,7 +9919,7 @@
         <v>38</v>
       </c>
       <c r="AE77" t="s" s="2">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="AF77" t="s" s="2">
         <v>39</v>
@@ -9937,15 +9934,15 @@
         <v>58</v>
       </c>
       <c r="AJ77" t="s" s="2">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="AK77" t="s" s="2">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="78" hidden="true">
       <c r="A78" t="s" s="2">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B78" s="2"/>
       <c r="C78" t="s" s="2">
@@ -10048,7 +10045,7 @@
     </row>
     <row r="79" hidden="true">
       <c r="A79" t="s" s="2">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B79" s="2"/>
       <c r="C79" t="s" s="2">
@@ -10153,7 +10150,7 @@
     </row>
     <row r="80" hidden="true">
       <c r="A80" t="s" s="2">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B80" s="2"/>
       <c r="C80" t="s" s="2">
@@ -10260,7 +10257,7 @@
     </row>
     <row r="81" hidden="true">
       <c r="A81" t="s" s="2">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B81" s="2"/>
       <c r="C81" t="s" s="2">
@@ -10363,7 +10360,7 @@
     </row>
     <row r="82" hidden="true">
       <c r="A82" t="s" s="2">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B82" s="2"/>
       <c r="C82" t="s" s="2">
@@ -10468,7 +10465,7 @@
     </row>
     <row r="83" hidden="true">
       <c r="A83" t="s" s="2">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B83" s="2"/>
       <c r="C83" t="s" s="2">
@@ -10510,7 +10507,7 @@
       </c>
       <c r="P83" s="2"/>
       <c r="Q83" t="s" s="2">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="R83" t="s" s="2">
         <v>38</v>
@@ -10575,7 +10572,7 @@
     </row>
     <row r="84" hidden="true">
       <c r="A84" t="s" s="2">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B84" s="2"/>
       <c r="C84" t="s" s="2">
@@ -10680,7 +10677,7 @@
     </row>
     <row r="85" hidden="true">
       <c r="A85" t="s" s="2">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B85" s="2"/>
       <c r="C85" t="s" s="2">
@@ -10785,7 +10782,7 @@
     </row>
     <row r="86" hidden="true">
       <c r="A86" t="s" s="2">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B86" s="2"/>
       <c r="C86" t="s" s="2">
@@ -10890,7 +10887,7 @@
     </row>
     <row r="87" hidden="true">
       <c r="A87" t="s" s="2">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B87" s="2"/>
       <c r="C87" t="s" s="2">
@@ -10997,7 +10994,7 @@
     </row>
     <row r="88" hidden="true">
       <c r="A88" t="s" s="2">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B88" s="2"/>
       <c r="C88" t="s" s="2">
@@ -11104,7 +11101,7 @@
     </row>
     <row r="89" hidden="true">
       <c r="A89" t="s" s="2">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B89" s="2"/>
       <c r="C89" t="s" s="2">
@@ -11127,17 +11124,17 @@
         <v>38</v>
       </c>
       <c r="J89" t="s" s="2">
+        <v>427</v>
+      </c>
+      <c r="K89" t="s" s="2">
         <v>428</v>
       </c>
-      <c r="K89" t="s" s="2">
+      <c r="L89" t="s" s="2">
         <v>429</v>
-      </c>
-      <c r="L89" t="s" s="2">
-        <v>430</v>
       </c>
       <c r="M89" s="2"/>
       <c r="N89" t="s" s="2">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="O89" t="s" s="2">
         <v>38</v>
@@ -11186,7 +11183,7 @@
         <v>38</v>
       </c>
       <c r="AE89" t="s" s="2">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="AF89" t="s" s="2">
         <v>39</v>
@@ -11201,7 +11198,7 @@
         <v>58</v>
       </c>
       <c r="AJ89" t="s" s="2">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="AK89" t="s" s="2">
         <v>38</v>
@@ -11209,7 +11206,7 @@
     </row>
     <row r="90" hidden="true">
       <c r="A90" t="s" s="2">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B90" s="2"/>
       <c r="C90" t="s" s="2">
@@ -11312,7 +11309,7 @@
     </row>
     <row r="91" hidden="true">
       <c r="A91" t="s" s="2">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B91" s="2"/>
       <c r="C91" t="s" s="2">
@@ -11417,11 +11414,11 @@
     </row>
     <row r="92" hidden="true">
       <c r="A92" t="s" s="2">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B92" s="2"/>
       <c r="C92" t="s" s="2">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D92" s="2"/>
       <c r="E92" t="s" s="2">
@@ -11443,10 +11440,10 @@
         <v>92</v>
       </c>
       <c r="K92" t="s" s="2">
+        <v>436</v>
+      </c>
+      <c r="L92" t="s" s="2">
         <v>437</v>
-      </c>
-      <c r="L92" t="s" s="2">
-        <v>438</v>
       </c>
       <c r="M92" t="s" s="2">
         <v>95</v>
@@ -11501,7 +11498,7 @@
         <v>38</v>
       </c>
       <c r="AE92" t="s" s="2">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="AF92" t="s" s="2">
         <v>39</v>
@@ -11524,7 +11521,7 @@
     </row>
     <row r="93" hidden="true">
       <c r="A93" t="s" s="2">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B93" s="2"/>
       <c r="C93" t="s" s="2">
@@ -11547,13 +11544,13 @@
         <v>38</v>
       </c>
       <c r="J93" t="s" s="2">
+        <v>440</v>
+      </c>
+      <c r="K93" t="s" s="2">
         <v>441</v>
       </c>
-      <c r="K93" t="s" s="2">
+      <c r="L93" t="s" s="2">
         <v>442</v>
-      </c>
-      <c r="L93" t="s" s="2">
-        <v>443</v>
       </c>
       <c r="M93" s="2"/>
       <c r="N93" s="2"/>
@@ -11604,7 +11601,7 @@
         <v>38</v>
       </c>
       <c r="AE93" t="s" s="2">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="AF93" t="s" s="2">
         <v>46</v>
@@ -11619,7 +11616,7 @@
         <v>58</v>
       </c>
       <c r="AJ93" t="s" s="2">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="AK93" t="s" s="2">
         <v>38</v>
@@ -11627,7 +11624,7 @@
     </row>
     <row r="94" hidden="true">
       <c r="A94" t="s" s="2">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B94" s="2"/>
       <c r="C94" t="s" s="2">
@@ -11650,13 +11647,13 @@
         <v>38</v>
       </c>
       <c r="J94" t="s" s="2">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="K94" t="s" s="2">
+        <v>445</v>
+      </c>
+      <c r="L94" t="s" s="2">
         <v>446</v>
-      </c>
-      <c r="L94" t="s" s="2">
-        <v>447</v>
       </c>
       <c r="M94" s="2"/>
       <c r="N94" s="2"/>
@@ -11707,7 +11704,7 @@
         <v>38</v>
       </c>
       <c r="AE94" t="s" s="2">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="AF94" t="s" s="2">
         <v>46</v>
@@ -11722,7 +11719,7 @@
         <v>58</v>
       </c>
       <c r="AJ94" t="s" s="2">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="AK94" t="s" s="2">
         <v>38</v>
@@ -11730,7 +11727,7 @@
     </row>
     <row r="95" hidden="true">
       <c r="A95" t="s" s="2">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B95" s="2"/>
       <c r="C95" t="s" s="2">
@@ -11753,13 +11750,13 @@
         <v>38</v>
       </c>
       <c r="J95" t="s" s="2">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="K95" t="s" s="2">
+        <v>448</v>
+      </c>
+      <c r="L95" t="s" s="2">
         <v>449</v>
-      </c>
-      <c r="L95" t="s" s="2">
-        <v>450</v>
       </c>
       <c r="M95" s="2"/>
       <c r="N95" s="2"/>
@@ -11810,7 +11807,7 @@
         <v>38</v>
       </c>
       <c r="AE95" t="s" s="2">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="AF95" t="s" s="2">
         <v>39</v>
@@ -11825,7 +11822,7 @@
         <v>58</v>
       </c>
       <c r="AJ95" t="s" s="2">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="AK95" t="s" s="2">
         <v>38</v>
@@ -11833,7 +11830,7 @@
     </row>
     <row r="96" hidden="true">
       <c r="A96" t="s" s="2">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B96" s="2"/>
       <c r="C96" t="s" s="2">
@@ -11856,19 +11853,19 @@
         <v>47</v>
       </c>
       <c r="J96" t="s" s="2">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="K96" t="s" s="2">
+        <v>451</v>
+      </c>
+      <c r="L96" t="s" s="2">
         <v>452</v>
       </c>
-      <c r="L96" t="s" s="2">
+      <c r="M96" t="s" s="2">
         <v>453</v>
       </c>
-      <c r="M96" t="s" s="2">
+      <c r="N96" t="s" s="2">
         <v>454</v>
-      </c>
-      <c r="N96" t="s" s="2">
-        <v>455</v>
       </c>
       <c r="O96" t="s" s="2">
         <v>38</v>
@@ -11917,7 +11914,7 @@
         <v>38</v>
       </c>
       <c r="AE96" t="s" s="2">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="AF96" t="s" s="2">
         <v>39</v>
@@ -11932,7 +11929,7 @@
         <v>58</v>
       </c>
       <c r="AJ96" t="s" s="2">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="AK96" t="s" s="2">
         <v>38</v>
@@ -11940,7 +11937,7 @@
     </row>
     <row r="97" hidden="true">
       <c r="A97" t="s" s="2">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B97" s="2"/>
       <c r="C97" t="s" s="2">
@@ -12043,7 +12040,7 @@
     </row>
     <row r="98" hidden="true">
       <c r="A98" t="s" s="2">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B98" s="2"/>
       <c r="C98" t="s" s="2">
@@ -12148,7 +12145,7 @@
     </row>
     <row r="99" hidden="true">
       <c r="A99" t="s" s="2">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B99" s="2"/>
       <c r="C99" t="s" s="2">
@@ -12174,13 +12171,13 @@
         <v>48</v>
       </c>
       <c r="K99" t="s" s="2">
+        <v>459</v>
+      </c>
+      <c r="L99" t="s" s="2">
         <v>460</v>
       </c>
-      <c r="L99" t="s" s="2">
+      <c r="M99" t="s" s="2">
         <v>461</v>
-      </c>
-      <c r="M99" t="s" s="2">
-        <v>462</v>
       </c>
       <c r="N99" s="2"/>
       <c r="O99" t="s" s="2">
@@ -12230,16 +12227,16 @@
         <v>38</v>
       </c>
       <c r="AE99" t="s" s="2">
+        <v>462</v>
+      </c>
+      <c r="AF99" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AG99" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="AH99" t="s" s="2">
         <v>463</v>
-      </c>
-      <c r="AF99" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AG99" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AH99" t="s" s="2">
-        <v>464</v>
       </c>
       <c r="AI99" t="s" s="2">
         <v>58</v>
@@ -12253,7 +12250,7 @@
     </row>
     <row r="100" hidden="true">
       <c r="A100" t="s" s="2">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B100" s="2"/>
       <c r="C100" t="s" s="2">
@@ -12279,13 +12276,13 @@
         <v>60</v>
       </c>
       <c r="K100" t="s" s="2">
+        <v>465</v>
+      </c>
+      <c r="L100" t="s" s="2">
         <v>466</v>
       </c>
-      <c r="L100" t="s" s="2">
+      <c r="M100" t="s" s="2">
         <v>467</v>
-      </c>
-      <c r="M100" t="s" s="2">
-        <v>468</v>
       </c>
       <c r="N100" s="2"/>
       <c r="O100" t="s" s="2">
@@ -12314,28 +12311,28 @@
         <v>137</v>
       </c>
       <c r="X100" t="s" s="2">
+        <v>468</v>
+      </c>
+      <c r="Y100" t="s" s="2">
         <v>469</v>
       </c>
-      <c r="Y100" t="s" s="2">
+      <c r="Z100" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AA100" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AB100" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AC100" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AD100" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AE100" t="s" s="2">
         <v>470</v>
-      </c>
-      <c r="Z100" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AA100" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AB100" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AC100" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AD100" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AE100" t="s" s="2">
-        <v>471</v>
       </c>
       <c r="AF100" t="s" s="2">
         <v>39</v>
@@ -12358,7 +12355,7 @@
     </row>
     <row r="101" hidden="true">
       <c r="A101" t="s" s="2">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B101" s="2"/>
       <c r="C101" t="s" s="2">
@@ -12384,13 +12381,13 @@
         <v>104</v>
       </c>
       <c r="K101" t="s" s="2">
+        <v>472</v>
+      </c>
+      <c r="L101" t="s" s="2">
         <v>473</v>
       </c>
-      <c r="L101" t="s" s="2">
+      <c r="M101" t="s" s="2">
         <v>474</v>
-      </c>
-      <c r="M101" t="s" s="2">
-        <v>475</v>
       </c>
       <c r="N101" s="2"/>
       <c r="O101" t="s" s="2">
@@ -12440,7 +12437,7 @@
         <v>38</v>
       </c>
       <c r="AE101" t="s" s="2">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="AF101" t="s" s="2">
         <v>39</v>
@@ -12455,7 +12452,7 @@
         <v>58</v>
       </c>
       <c r="AJ101" t="s" s="2">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="AK101" t="s" s="2">
         <v>38</v>
@@ -12463,7 +12460,7 @@
     </row>
     <row r="102" hidden="true">
       <c r="A102" t="s" s="2">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B102" s="2"/>
       <c r="C102" t="s" s="2">
@@ -12489,13 +12486,13 @@
         <v>48</v>
       </c>
       <c r="K102" t="s" s="2">
+        <v>478</v>
+      </c>
+      <c r="L102" t="s" s="2">
         <v>479</v>
       </c>
-      <c r="L102" t="s" s="2">
+      <c r="M102" t="s" s="2">
         <v>480</v>
-      </c>
-      <c r="M102" t="s" s="2">
-        <v>481</v>
       </c>
       <c r="N102" s="2"/>
       <c r="O102" t="s" s="2">
@@ -12545,7 +12542,7 @@
         <v>38</v>
       </c>
       <c r="AE102" t="s" s="2">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="AF102" t="s" s="2">
         <v>39</v>
@@ -12568,7 +12565,7 @@
     </row>
     <row r="103" hidden="true">
       <c r="A103" t="s" s="2">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B103" s="2"/>
       <c r="C103" t="s" s="2">
@@ -12591,17 +12588,17 @@
         <v>38</v>
       </c>
       <c r="J103" t="s" s="2">
+        <v>483</v>
+      </c>
+      <c r="K103" t="s" s="2">
         <v>484</v>
       </c>
-      <c r="K103" t="s" s="2">
+      <c r="L103" t="s" s="2">
         <v>485</v>
-      </c>
-      <c r="L103" t="s" s="2">
-        <v>486</v>
       </c>
       <c r="M103" s="2"/>
       <c r="N103" t="s" s="2">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="O103" t="s" s="2">
         <v>38</v>
@@ -12650,7 +12647,7 @@
         <v>38</v>
       </c>
       <c r="AE103" t="s" s="2">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="AF103" t="s" s="2">
         <v>39</v>
@@ -12665,7 +12662,7 @@
         <v>58</v>
       </c>
       <c r="AJ103" t="s" s="2">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="AK103" t="s" s="2">
         <v>38</v>
@@ -12673,7 +12670,7 @@
     </row>
     <row r="104" hidden="true">
       <c r="A104" t="s" s="2">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B104" s="2"/>
       <c r="C104" t="s" s="2">
@@ -12776,7 +12773,7 @@
     </row>
     <row r="105" hidden="true">
       <c r="A105" t="s" s="2">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B105" s="2"/>
       <c r="C105" t="s" s="2">
@@ -12881,7 +12878,7 @@
     </row>
     <row r="106" hidden="true">
       <c r="A106" t="s" s="2">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B106" s="2"/>
       <c r="C106" t="s" s="2">
@@ -12907,13 +12904,13 @@
         <v>48</v>
       </c>
       <c r="K106" t="s" s="2">
+        <v>459</v>
+      </c>
+      <c r="L106" t="s" s="2">
         <v>460</v>
       </c>
-      <c r="L106" t="s" s="2">
-        <v>461</v>
-      </c>
       <c r="M106" t="s" s="2">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="N106" s="2"/>
       <c r="O106" t="s" s="2">
@@ -12963,16 +12960,16 @@
         <v>38</v>
       </c>
       <c r="AE106" t="s" s="2">
+        <v>462</v>
+      </c>
+      <c r="AF106" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AG106" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="AH106" t="s" s="2">
         <v>463</v>
-      </c>
-      <c r="AF106" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AG106" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AH106" t="s" s="2">
-        <v>464</v>
       </c>
       <c r="AI106" t="s" s="2">
         <v>58</v>
@@ -12986,7 +12983,7 @@
     </row>
     <row r="107" hidden="true">
       <c r="A107" t="s" s="2">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B107" s="2"/>
       <c r="C107" t="s" s="2">
@@ -13012,13 +13009,13 @@
         <v>60</v>
       </c>
       <c r="K107" t="s" s="2">
+        <v>465</v>
+      </c>
+      <c r="L107" t="s" s="2">
         <v>466</v>
       </c>
-      <c r="L107" t="s" s="2">
+      <c r="M107" t="s" s="2">
         <v>467</v>
-      </c>
-      <c r="M107" t="s" s="2">
-        <v>468</v>
       </c>
       <c r="N107" s="2"/>
       <c r="O107" t="s" s="2">
@@ -13047,28 +13044,28 @@
         <v>137</v>
       </c>
       <c r="X107" t="s" s="2">
+        <v>468</v>
+      </c>
+      <c r="Y107" t="s" s="2">
         <v>469</v>
       </c>
-      <c r="Y107" t="s" s="2">
+      <c r="Z107" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AA107" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AB107" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AC107" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AD107" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AE107" t="s" s="2">
         <v>470</v>
-      </c>
-      <c r="Z107" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AA107" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AB107" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AC107" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AD107" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AE107" t="s" s="2">
-        <v>471</v>
       </c>
       <c r="AF107" t="s" s="2">
         <v>39</v>
@@ -13091,7 +13088,7 @@
     </row>
     <row r="108" hidden="true">
       <c r="A108" t="s" s="2">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B108" s="2"/>
       <c r="C108" t="s" s="2">
@@ -13117,13 +13114,13 @@
         <v>104</v>
       </c>
       <c r="K108" t="s" s="2">
+        <v>472</v>
+      </c>
+      <c r="L108" t="s" s="2">
         <v>473</v>
       </c>
-      <c r="L108" t="s" s="2">
+      <c r="M108" t="s" s="2">
         <v>474</v>
-      </c>
-      <c r="M108" t="s" s="2">
-        <v>475</v>
       </c>
       <c r="N108" s="2"/>
       <c r="O108" t="s" s="2">
@@ -13173,7 +13170,7 @@
         <v>38</v>
       </c>
       <c r="AE108" t="s" s="2">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="AF108" t="s" s="2">
         <v>39</v>
@@ -13188,7 +13185,7 @@
         <v>58</v>
       </c>
       <c r="AJ108" t="s" s="2">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="AK108" t="s" s="2">
         <v>38</v>
@@ -13196,7 +13193,7 @@
     </row>
     <row r="109" hidden="true">
       <c r="A109" t="s" s="2">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B109" s="2"/>
       <c r="C109" t="s" s="2">
@@ -13222,13 +13219,13 @@
         <v>48</v>
       </c>
       <c r="K109" t="s" s="2">
+        <v>478</v>
+      </c>
+      <c r="L109" t="s" s="2">
         <v>479</v>
       </c>
-      <c r="L109" t="s" s="2">
+      <c r="M109" t="s" s="2">
         <v>480</v>
-      </c>
-      <c r="M109" t="s" s="2">
-        <v>481</v>
       </c>
       <c r="N109" s="2"/>
       <c r="O109" t="s" s="2">
@@ -13278,7 +13275,7 @@
         <v>38</v>
       </c>
       <c r="AE109" t="s" s="2">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="AF109" t="s" s="2">
         <v>39</v>
@@ -13301,7 +13298,7 @@
     </row>
     <row r="110" hidden="true">
       <c r="A110" t="s" s="2">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B110" s="2"/>
       <c r="C110" t="s" s="2">
@@ -13324,16 +13321,16 @@
         <v>38</v>
       </c>
       <c r="J110" t="s" s="2">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="K110" t="s" s="2">
+        <v>496</v>
+      </c>
+      <c r="L110" t="s" s="2">
         <v>497</v>
       </c>
-      <c r="L110" t="s" s="2">
+      <c r="M110" t="s" s="2">
         <v>498</v>
-      </c>
-      <c r="M110" t="s" s="2">
-        <v>499</v>
       </c>
       <c r="N110" s="2"/>
       <c r="O110" t="s" s="2">
@@ -13383,7 +13380,7 @@
         <v>38</v>
       </c>
       <c r="AE110" t="s" s="2">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="AF110" t="s" s="2">
         <v>39</v>
@@ -13398,7 +13395,7 @@
         <v>58</v>
       </c>
       <c r="AJ110" t="s" s="2">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="AK110" t="s" s="2">
         <v>38</v>
@@ -13406,7 +13403,7 @@
     </row>
     <row r="111" hidden="true">
       <c r="A111" t="s" s="2">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B111" s="2"/>
       <c r="C111" t="s" s="2">
@@ -13509,7 +13506,7 @@
     </row>
     <row r="112" hidden="true">
       <c r="A112" t="s" s="2">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B112" s="2"/>
       <c r="C112" t="s" s="2">
@@ -13614,11 +13611,11 @@
     </row>
     <row r="113" hidden="true">
       <c r="A113" t="s" s="2">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B113" s="2"/>
       <c r="C113" t="s" s="2">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D113" s="2"/>
       <c r="E113" t="s" s="2">
@@ -13640,10 +13637,10 @@
         <v>92</v>
       </c>
       <c r="K113" t="s" s="2">
+        <v>436</v>
+      </c>
+      <c r="L113" t="s" s="2">
         <v>437</v>
-      </c>
-      <c r="L113" t="s" s="2">
-        <v>438</v>
       </c>
       <c r="M113" t="s" s="2">
         <v>95</v>
@@ -13698,7 +13695,7 @@
         <v>38</v>
       </c>
       <c r="AE113" t="s" s="2">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="AF113" t="s" s="2">
         <v>39</v>
@@ -13721,7 +13718,7 @@
     </row>
     <row r="114" hidden="true">
       <c r="A114" t="s" s="2">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B114" s="2"/>
       <c r="C114" t="s" s="2">
@@ -13747,10 +13744,10 @@
         <v>66</v>
       </c>
       <c r="K114" t="s" s="2">
+        <v>504</v>
+      </c>
+      <c r="L114" t="s" s="2">
         <v>505</v>
-      </c>
-      <c r="L114" t="s" s="2">
-        <v>506</v>
       </c>
       <c r="M114" s="2"/>
       <c r="N114" s="2"/>
@@ -13780,11 +13777,11 @@
         <v>126</v>
       </c>
       <c r="X114" t="s" s="2">
+        <v>506</v>
+      </c>
+      <c r="Y114" t="s" s="2">
         <v>507</v>
       </c>
-      <c r="Y114" t="s" s="2">
-        <v>508</v>
-      </c>
       <c r="Z114" t="s" s="2">
         <v>38</v>
       </c>
@@ -13801,7 +13798,7 @@
         <v>38</v>
       </c>
       <c r="AE114" t="s" s="2">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="AF114" t="s" s="2">
         <v>39</v>
@@ -13816,7 +13813,7 @@
         <v>58</v>
       </c>
       <c r="AJ114" t="s" s="2">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="AK114" t="s" s="2">
         <v>38</v>
@@ -13824,7 +13821,7 @@
     </row>
     <row r="115" hidden="true">
       <c r="A115" t="s" s="2">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B115" s="2"/>
       <c r="C115" t="s" s="2">
@@ -13850,10 +13847,10 @@
         <v>179</v>
       </c>
       <c r="K115" t="s" s="2">
+        <v>509</v>
+      </c>
+      <c r="L115" t="s" s="2">
         <v>510</v>
-      </c>
-      <c r="L115" t="s" s="2">
-        <v>511</v>
       </c>
       <c r="M115" s="2"/>
       <c r="N115" s="2"/>
@@ -13904,7 +13901,7 @@
         <v>38</v>
       </c>
       <c r="AE115" t="s" s="2">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="AF115" t="s" s="2">
         <v>39</v>
@@ -13919,7 +13916,7 @@
         <v>58</v>
       </c>
       <c r="AJ115" t="s" s="2">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="AK115" t="s" s="2">
         <v>38</v>
@@ -13927,7 +13924,7 @@
     </row>
     <row r="116" hidden="true">
       <c r="A116" t="s" s="2">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B116" s="2"/>
       <c r="C116" t="s" s="2">
@@ -13950,13 +13947,13 @@
         <v>38</v>
       </c>
       <c r="J116" t="s" s="2">
+        <v>512</v>
+      </c>
+      <c r="K116" t="s" s="2">
         <v>513</v>
       </c>
-      <c r="K116" t="s" s="2">
+      <c r="L116" t="s" s="2">
         <v>514</v>
-      </c>
-      <c r="L116" t="s" s="2">
-        <v>515</v>
       </c>
       <c r="M116" s="2"/>
       <c r="N116" s="2"/>
@@ -14007,7 +14004,7 @@
         <v>38</v>
       </c>
       <c r="AE116" t="s" s="2">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="AF116" t="s" s="2">
         <v>39</v>
@@ -14022,7 +14019,7 @@
         <v>58</v>
       </c>
       <c r="AJ116" t="s" s="2">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="AK116" t="s" s="2">
         <v>38</v>
@@ -14030,7 +14027,7 @@
     </row>
     <row r="117" hidden="true">
       <c r="A117" t="s" s="2">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B117" s="2"/>
       <c r="C117" t="s" s="2">
@@ -14053,13 +14050,13 @@
         <v>38</v>
       </c>
       <c r="J117" t="s" s="2">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="K117" t="s" s="2">
+        <v>516</v>
+      </c>
+      <c r="L117" t="s" s="2">
         <v>517</v>
-      </c>
-      <c r="L117" t="s" s="2">
-        <v>518</v>
       </c>
       <c r="M117" s="2"/>
       <c r="N117" s="2"/>
@@ -14110,7 +14107,7 @@
         <v>38</v>
       </c>
       <c r="AE117" t="s" s="2">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="AF117" t="s" s="2">
         <v>39</v>
@@ -14125,7 +14122,7 @@
         <v>58</v>
       </c>
       <c r="AJ117" t="s" s="2">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="AK117" t="s" s="2">
         <v>38</v>
@@ -14133,7 +14130,7 @@
     </row>
     <row r="118" hidden="true">
       <c r="A118" t="s" s="2">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B118" s="2"/>
       <c r="C118" t="s" s="2">
@@ -14159,10 +14156,10 @@
         <v>48</v>
       </c>
       <c r="K118" t="s" s="2">
+        <v>519</v>
+      </c>
+      <c r="L118" t="s" s="2">
         <v>520</v>
-      </c>
-      <c r="L118" t="s" s="2">
-        <v>521</v>
       </c>
       <c r="M118" s="2"/>
       <c r="N118" s="2"/>
@@ -14213,7 +14210,7 @@
         <v>38</v>
       </c>
       <c r="AE118" t="s" s="2">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="AF118" t="s" s="2">
         <v>39</v>
@@ -14236,7 +14233,7 @@
     </row>
     <row r="119" hidden="true">
       <c r="A119" t="s" s="2">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B119" s="2"/>
       <c r="C119" t="s" s="2">
@@ -14259,17 +14256,17 @@
         <v>38</v>
       </c>
       <c r="J119" t="s" s="2">
+        <v>522</v>
+      </c>
+      <c r="K119" t="s" s="2">
         <v>523</v>
       </c>
-      <c r="K119" t="s" s="2">
+      <c r="L119" t="s" s="2">
         <v>524</v>
-      </c>
-      <c r="L119" t="s" s="2">
-        <v>525</v>
       </c>
       <c r="M119" s="2"/>
       <c r="N119" t="s" s="2">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="O119" t="s" s="2">
         <v>38</v>
@@ -14318,7 +14315,7 @@
         <v>38</v>
       </c>
       <c r="AE119" t="s" s="2">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="AF119" t="s" s="2">
         <v>39</v>

</xml_diff>